<commit_message>
Open PDF in binary
</commit_message>
<xml_diff>
--- a/tmp/table.xlsx
+++ b/tmp/table.xlsx
@@ -436,17 +436,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Alice</t>
+          <t>Kate</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bob</t>
+          <t>Danil</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>